<commit_message>
actualización estable de Python con Merma ajustada solo a productos pigmentadosV2 cotejada con Luchis
</commit_message>
<xml_diff>
--- a/LS_BASE.xlsx
+++ b/LS_BASE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bam/Documents/WorkWork/GrupoLaser/Dir_Gen/A_Comercial/Listas_Precios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1A6BBD-B6BD-0F44-A2EE-0319B1B0B2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933AB694-E0E3-DF47-994A-ADE14AA375ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="7840" windowWidth="27640" windowHeight="16940" xr2:uid="{E9ADC6AB-4182-2F4C-A392-507D92B497BE}"/>
+    <workbookView xWindow="3480" yWindow="2280" windowWidth="27640" windowHeight="16940" xr2:uid="{E9ADC6AB-4182-2F4C-A392-507D92B497BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" r:id="rId1"/>
@@ -7597,8 +7597,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
@@ -7650,12 +7651,12 @@
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -7663,17 +7664,18 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
+    <cellStyle name="Comma" xfId="5" builtinId="3"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Moneda 2" xfId="4" xr:uid="{DD1B5AEB-A02A-464F-AB41-30CBA57525BF}"/>
+    <cellStyle name="Moneda 2" xfId="3" xr:uid="{DD1B5AEB-A02A-464F-AB41-30CBA57525BF}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5" xr:uid="{F0F36339-0A5E-7243-9328-54F105A92016}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{1F872AAA-4A2B-9648-A5EB-9BB162F8EC54}"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{F0F36339-0A5E-7243-9328-54F105A92016}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{1F872AAA-4A2B-9648-A5EB-9BB162F8EC54}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -8276,8 +8278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E049D776-D817-6E4D-B3A4-91727BF98221}">
   <dimension ref="A1:J1200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8288,8 +8290,8 @@
     <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.1640625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -8313,10 +8315,10 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="8" t="s">
         <v>2512</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="8" t="s">
         <v>2513</v>
       </c>
       <c r="I1" t="s">

</xml_diff>